<commit_message>
eg3 grid 0.5 and 0.25
</commit_message>
<xml_diff>
--- a/eg1 adavanced.xlsx
+++ b/eg1 adavanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiqing/Desktop/Lipschitz-System-ID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060243DA-C428-E94C-A5CF-B1D10A4EF33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E23000-5051-C34E-A6B4-FD782CECD9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="5" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
   </bookViews>
   <sheets>
     <sheet name="Ours 0.25" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -153,9 +153,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7B8AE4-A984-5E47-83F5-2F9341F82724}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f t="shared" ref="A28:M32" ca="1" si="1">AVERAGE(OFFSET(A$2,(ROW()-27)*4,0,4,1))</f>
+        <f t="shared" ref="A28:A31" ca="1" si="1">AVERAGE(OFFSET(A$2,(ROW()-27)*4,0,4,1))</f>
         <v>1</v>
       </c>
       <c r="B28" s="9">
@@ -1696,55 +1696,55 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="4">
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>7.1235152773876107E-3</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="10">
         <f t="shared" ca="1" si="0"/>
         <v>7.0908442065317845E-3</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <f t="shared" ca="1" si="0"/>
         <v>58.75</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="4">
         <f t="shared" ca="1" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="7">
         <f t="shared" ca="1" si="0"/>
         <v>8.0150671005249006</v>
       </c>
-      <c r="G30" s="6" t="e">
+      <c r="G30" s="7" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="7">
         <f t="shared" ca="1" si="0"/>
         <v>9.7557201236299296</v>
       </c>
-      <c r="I30" s="6" t="e">
+      <c r="I30" s="7" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="7">
         <f t="shared" ca="1" si="0"/>
         <v>6.9822730168608977</v>
       </c>
-      <c r="K30" s="6" t="e">
+      <c r="K30" s="7" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L30" s="6">
+      <c r="L30" s="7">
         <f t="shared" ca="1" si="0"/>
         <v>5.4388422338016174</v>
       </c>
-      <c r="M30" s="6" t="e">
+      <c r="M30" s="7" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1855,6 +1855,12 @@
       <c r="M32" s="6" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="9">
+        <f ca="1">MIN(C27:C32)</f>
+        <v>7.0908442065317845E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1865,9 +1871,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4411848-26EC-7848-88E5-EF7373A463AB}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:M29"/>
     </sheetView>
   </sheetViews>
@@ -3121,55 +3127,55 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="4">
         <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="10">
         <f t="shared" ca="1" si="1"/>
         <v>7.0832125233248455E-3</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="10">
         <f t="shared" ca="1" si="1"/>
         <v>7.0098088323534927E-3</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <f t="shared" ca="1" si="1"/>
         <v>76.25</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="7">
         <f t="shared" ca="1" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="7">
         <f t="shared" ca="1" si="1"/>
         <v>16.030134201049801</v>
       </c>
-      <c r="G31" s="6" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H31" s="6">
+      <c r="G31" s="7" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="7">
         <f t="shared" ca="1" si="1"/>
         <v>17.509938044629525</v>
       </c>
-      <c r="I31" s="6" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J31" s="6">
+      <c r="I31" s="7" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31" s="7">
         <f t="shared" ca="1" si="1"/>
         <v>11.729536304052626</v>
       </c>
-      <c r="K31" s="6" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L31" s="6">
+      <c r="K31" s="7" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" s="7">
         <f t="shared" ca="1" si="1"/>
         <v>9.3502520081546585</v>
       </c>
-      <c r="M31" s="6" t="e">
+      <c r="M31" s="7" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -3226,6 +3232,12 @@
       <c r="M32" s="6" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="9">
+        <f ca="1">MIN(C27:C32)</f>
+        <v>7.0098088323534927E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3235,10 +3247,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C910F4E5-1871-5D44-A4D1-B4921F11A929}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4596,6 +4608,12 @@
       <c r="M32" s="6" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="9">
+        <f ca="1">MIN(C27:C32)</f>
+        <v>6.9671547129512394E-3</v>
       </c>
     </row>
   </sheetData>
@@ -5973,433 +5991,433 @@
     </row>
     <row r="35" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ref="A35:A42" ca="1" si="0">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
         <v>1E-8</v>
       </c>
       <c r="B35" s="11">
-        <f t="shared" ref="B35:M42" ca="1" si="0">AVERAGE(OFFSET(B$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ref="B35:M42" ca="1" si="1">AVERAGE(OFFSET(B$2,(ROW()-35)*4,0,4,1))</f>
         <v>7.2448755443551846E-3</v>
       </c>
       <c r="C35" s="11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.187035253043577E-3</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>96.25</v>
       </c>
       <c r="E35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>30.337723255157428</v>
       </c>
       <c r="G35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>8.3969376329842262</v>
       </c>
       <c r="H35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>31.370526435434424</v>
       </c>
       <c r="I35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>10.126425754002927</v>
       </c>
       <c r="J35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>20.578242454387102</v>
       </c>
       <c r="K35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.1553661932995531</v>
       </c>
       <c r="L35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>15.996092140658423</v>
       </c>
       <c r="M35" s="8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>5.6868486828285425</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B36" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.2402143367922799E-3</v>
       </c>
       <c r="C36" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.1886290692070353E-3</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>98.75</v>
       </c>
       <c r="E36" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F36" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>29.636587619781427</v>
       </c>
       <c r="G36" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H36" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I36" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J36" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K36" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L36" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M36" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="B37" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.2558131985405953E-3</v>
       </c>
       <c r="C37" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.1959295310080025E-3</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>101.25</v>
       </c>
       <c r="E37" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F37" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>27.604599475860525</v>
       </c>
       <c r="G37" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H37" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I37" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J37" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K37" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L37" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M37" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="B38" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.2538787907762223E-3</v>
       </c>
       <c r="C38" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.2017070760534299E-3</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>103.75</v>
       </c>
       <c r="E38" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F38" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>25.570649623870803</v>
       </c>
       <c r="G38" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H38" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J38" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K38" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L38" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M38" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1E-4</v>
       </c>
       <c r="B39" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.2755244030478427E-3</v>
       </c>
       <c r="C39" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.207872814181792E-3</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>106.25</v>
       </c>
       <c r="E39" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>21.7788982391357</v>
       </c>
       <c r="G39" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H39" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I39" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J39" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K39" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L39" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M39" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="B40" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.3679907190454877E-3</v>
       </c>
       <c r="C40" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.3069674247737051E-3</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>108.75</v>
       </c>
       <c r="E40" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>13.705420494079524</v>
       </c>
       <c r="G40" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H40" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I40" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J40" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K40" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L40" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M40" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.01</v>
       </c>
       <c r="B41" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.9807669067993078E-3</v>
       </c>
       <c r="C41" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.9187246638924812E-3</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>111.25</v>
       </c>
       <c r="E41" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F41" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>7.5595898628234828</v>
       </c>
       <c r="G41" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H41" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I41" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J41" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K41" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L41" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M41" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <f ca="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.1</v>
       </c>
       <c r="B42" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>3.9111126818399207</v>
       </c>
       <c r="C42" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>3.8345109020233394</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>113.75</v>
       </c>
       <c r="E42" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F42" s="6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>4.5242187976837123</v>
       </c>
       <c r="G42" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H42" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I42" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J42" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K42" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L42" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M42" s="6" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8232,7 +8250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9902717B-D473-4C4C-BD56-0A1D1459D334}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -10048,7 +10066,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:M41"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11472,7 +11490,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <f t="shared" ref="A36:M43" ca="1" si="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
+        <f t="shared" ref="A36:M42" ca="1" si="1">AVERAGE(OFFSET(A$2,(ROW()-35)*4,0,4,1))</f>
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="B36" s="9">

</xml_diff>

<commit_message>
eg1 eg2 eg3 get_estimate_error
</commit_message>
<xml_diff>
--- a/eg1 adavanced.xlsx
+++ b/eg1 adavanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiqing/Desktop/Lipschitz-System-ID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E23000-5051-C34E-A6B4-FD782CECD9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB27A79-1EA5-B74F-812F-72A9438D35D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
+    <workbookView xWindow="52500" yWindow="4220" windowWidth="34560" windowHeight="19800" xr2:uid="{624D5C9E-D399-6E42-9BAD-9829FF00FD61}"/>
   </bookViews>
   <sheets>
     <sheet name="Ours 0.25" sheetId="1" r:id="rId1"/>
@@ -8250,7 +8250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9902717B-D473-4C4C-BD56-0A1D1459D334}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>